<commit_message>
Update ps value for L1_SingleMu7
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v1_3_0/PrescaleTable/L1Menu_Collisions2022_v1_3_0-DedicatedRateStudyRun3.xlsx
+++ b/development/L1Menu_Collisions2022_v1_3_0/PrescaleTable/L1Menu_Collisions2022_v1_3_0-DedicatedRateStudyRun3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2022_v1_3_0/PrescaleTable/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBCBBA8-2987-2F44-BBB2-18B4F5A48F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6307BDBD-9CF2-D544-9595-7D698852C321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2500" yWindow="-17280" windowWidth="27840" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1647,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R404"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
-      <selection activeCell="B299" sqref="B299"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2395,49 +2395,49 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="F14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="G14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="H14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="I14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="J14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="K14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="L14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="M14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="N14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="O14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="P14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="Q14">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="R14">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>